<commit_message>
Added MY document type for busdox; TICC-328
</commit_message>
<xml_diff>
--- a/publication/v8.8/Peppol Code Lists - Document types v8.8.xlsx
+++ b/publication/v8.8/Peppol Code Lists - Document types v8.8.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\edec-codelists\work-in-progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD45B871-85A7-4D72-B83D-6F2AC92349EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{253111BE-14E4-4C40-8BFF-9403C43F0C19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1915" uniqueCount="670">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1947" uniqueCount="671">
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:ApplicationResponse-2::ApplicationResponse##urn:www.cenbii.eu:transaction:biicoretrdm057:ver1.0:#urn:www.peppol.eu:bis:peppol1a:ver1.0::2.0</t>
   </si>
@@ -2098,6 +2098,9 @@
   </si>
   <si>
     <t>TICC-312</t>
+  </si>
+  <si>
+    <t>TICC-328</t>
   </si>
 </sst>
 </file>
@@ -2757,10 +2760,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F45987FB-91F4-488D-A9D3-2F3FAED3E07C}">
-  <dimension ref="A1:L249"/>
+  <dimension ref="A1:L253"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A234" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A237" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A250" sqref="A250"/>
     </sheetView>
   </sheetViews>
@@ -10690,6 +10693,134 @@
         <v>532</v>
       </c>
     </row>
+    <row r="250" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
+        <v>661</v>
+      </c>
+      <c r="B250" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C250" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="D250" s="29" t="s">
+        <v>659</v>
+      </c>
+      <c r="E250" s="24" t="s">
+        <v>367</v>
+      </c>
+      <c r="H250" s="5" t="s">
+        <v>670</v>
+      </c>
+      <c r="I250" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J250" s="24">
+        <v>3</v>
+      </c>
+      <c r="K250" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="L250" s="5" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="251" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>662</v>
+      </c>
+      <c r="B251" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C251" s="1" t="s">
+        <v>666</v>
+      </c>
+      <c r="D251" s="29" t="s">
+        <v>659</v>
+      </c>
+      <c r="E251" s="24" t="s">
+        <v>367</v>
+      </c>
+      <c r="H251" s="5" t="s">
+        <v>670</v>
+      </c>
+      <c r="I251" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J251" s="24">
+        <v>3</v>
+      </c>
+      <c r="K251" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="L251" s="5" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="252" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>663</v>
+      </c>
+      <c r="B252" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C252" s="1" t="s">
+        <v>667</v>
+      </c>
+      <c r="D252" s="29" t="s">
+        <v>659</v>
+      </c>
+      <c r="E252" s="24" t="s">
+        <v>367</v>
+      </c>
+      <c r="H252" s="5" t="s">
+        <v>670</v>
+      </c>
+      <c r="I252" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J252" s="24">
+        <v>3</v>
+      </c>
+      <c r="K252" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="L252" s="5" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="253" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
+        <v>664</v>
+      </c>
+      <c r="B253" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C253" s="1" t="s">
+        <v>668</v>
+      </c>
+      <c r="D253" s="29" t="s">
+        <v>659</v>
+      </c>
+      <c r="E253" s="24" t="s">
+        <v>367</v>
+      </c>
+      <c r="H253" s="5" t="s">
+        <v>670</v>
+      </c>
+      <c r="I253" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J253" s="24">
+        <v>3</v>
+      </c>
+      <c r="K253" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="L253" s="5" t="s">
+        <v>532</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:L245" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>